<commit_message>
avance de ingreso con parcela
</commit_message>
<xml_diff>
--- a/Plantillas/plantilla_socios.xlsx
+++ b/Plantillas/plantilla_socios.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sctock_camu\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41762A60-BB7E-4B4E-A4F3-1A7E5A955306}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553691AA-5636-4098-97FC-9CB01FD3BD1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$68</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
@@ -1240,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q68"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:R1048576"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2958,6 +2961,7 @@
       <c r="I68" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I68" xr:uid="{FE01B379-5120-4C48-B557-ACAD04822C99}"/>
   <dataValidations count="1">
     <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor inválido" error="Solo se permite 0 o 1." sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"0,1"</formula1>

</xml_diff>